<commit_message>
Badge Adding Conditon Added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
+++ b/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="315">
   <si>
     <t>FirstName</t>
   </si>
@@ -876,6 +876,96 @@
   </si>
   <si>
     <t>AssignmentName40482</t>
+  </si>
+  <si>
+    <t>PortfolioCourse87630</t>
+  </si>
+  <si>
+    <t>AssignmentName87630</t>
+  </si>
+  <si>
+    <t>PortfolioCourse71875</t>
+  </si>
+  <si>
+    <t>AssignmentName71875</t>
+  </si>
+  <si>
+    <t>PortfolioCourse86669</t>
+  </si>
+  <si>
+    <t>AssignmentName86669</t>
+  </si>
+  <si>
+    <t>PortfolioCourse16893</t>
+  </si>
+  <si>
+    <t>AssignmentName16893</t>
+  </si>
+  <si>
+    <t>PortfolioCourse88270</t>
+  </si>
+  <si>
+    <t>AssignmentName88270</t>
+  </si>
+  <si>
+    <t>PortfolioCourse88475</t>
+  </si>
+  <si>
+    <t>AssignmentName88475</t>
+  </si>
+  <si>
+    <t>PortfolioCourse73066</t>
+  </si>
+  <si>
+    <t>AssignmentName73066</t>
+  </si>
+  <si>
+    <t>PortfolioCourse56184</t>
+  </si>
+  <si>
+    <t>AssignmentName56184</t>
+  </si>
+  <si>
+    <t>PortfolioCourse53718</t>
+  </si>
+  <si>
+    <t>AssignmentName53718</t>
+  </si>
+  <si>
+    <t>PortfolioCourse90775</t>
+  </si>
+  <si>
+    <t>AssignmentName90775</t>
+  </si>
+  <si>
+    <t>PortfolioCourse84615</t>
+  </si>
+  <si>
+    <t>AssignmentName84615</t>
+  </si>
+  <si>
+    <t>PortfolioCourse40267</t>
+  </si>
+  <si>
+    <t>AssignmentName40267</t>
+  </si>
+  <si>
+    <t>PortfolioCourse44425</t>
+  </si>
+  <si>
+    <t>AssignmentName44425</t>
+  </si>
+  <si>
+    <t>PortfolioCourse52667</t>
+  </si>
+  <si>
+    <t>AssignmentName52667</t>
+  </si>
+  <si>
+    <t>PortfolioCourse47023</t>
+  </si>
+  <si>
+    <t>AssignmentName47023</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,6 +1171,96 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -2134,11 +2314,11 @@
       <c r="L2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s" s="232">
-        <v>283</v>
-      </c>
-      <c r="N2" t="s" s="233">
-        <v>284</v>
+      <c r="M2" t="s" s="262">
+        <v>313</v>
+      </c>
+      <c r="N2" t="s" s="263">
+        <v>314</v>
       </c>
       <c r="O2" t="s" s="230">
         <v>281</v>

</xml_diff>

<commit_message>
Logic Changed for Badge Xpath
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
+++ b/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="351">
   <si>
     <t>FirstName</t>
   </si>
@@ -1068,6 +1068,12 @@
   </si>
   <si>
     <t>AssignmentName65242</t>
+  </si>
+  <si>
+    <t>PortfolioCourse82107</t>
+  </si>
+  <si>
+    <t>AssignmentName82107</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="298">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1273,6 +1279,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -2518,11 +2530,11 @@
       <c r="L2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s" s="296">
-        <v>347</v>
-      </c>
-      <c r="N2" t="s" s="297">
-        <v>348</v>
+      <c r="M2" t="s" s="298">
+        <v>349</v>
+      </c>
+      <c r="N2" t="s" s="299">
+        <v>350</v>
       </c>
       <c r="O2" t="s" s="230">
         <v>281</v>

</xml_diff>

<commit_message>
Course Xpath's Updated and Loop Count Increased
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
+++ b/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
   <si>
     <t>FirstName</t>
   </si>
@@ -439,6 +439,18 @@
   </si>
   <si>
     <t>AssignmentName97496</t>
+  </si>
+  <si>
+    <t>PortfolioCourse43630</t>
+  </si>
+  <si>
+    <t>AssignmentName43630</t>
+  </si>
+  <si>
+    <t>PortfolioCourse62144</t>
+  </si>
+  <si>
+    <t>AssignmentName62144</t>
   </si>
 </sst>
 </file>
@@ -584,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -644,6 +656,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1253,17 +1277,17 @@
       <c r="L2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s" s="82">
-        <v>135</v>
-      </c>
-      <c r="N2" t="s" s="83">
-        <v>136</v>
-      </c>
-      <c r="O2" t="s" s="84">
-        <v>137</v>
-      </c>
-      <c r="P2" t="s" s="85">
-        <v>138</v>
+      <c r="M2" t="s" s="86">
+        <v>139</v>
+      </c>
+      <c r="N2" t="s" s="87">
+        <v>140</v>
+      </c>
+      <c r="O2" t="s" s="88">
+        <v>141</v>
+      </c>
+      <c r="P2" t="s" s="89">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Latest Script and Badge related Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
+++ b/src/test/resources/ExcelFiles/PortfolioCenter.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t>FirstName</t>
   </si>
@@ -205,6 +205,150 @@
   </si>
   <si>
     <t>AssignmentName11152</t>
+  </si>
+  <si>
+    <t>PortfolioCourse46050</t>
+  </si>
+  <si>
+    <t>AssignmentName46050</t>
+  </si>
+  <si>
+    <t>PortfolioCourse46818</t>
+  </si>
+  <si>
+    <t>AssignmentName46818</t>
+  </si>
+  <si>
+    <t>PortfolioCourse50318</t>
+  </si>
+  <si>
+    <t>AssignmentName50318</t>
+  </si>
+  <si>
+    <t>PortfolioCourse24046</t>
+  </si>
+  <si>
+    <t>AssignmentName24046</t>
+  </si>
+  <si>
+    <t>PortfolioCourse74026</t>
+  </si>
+  <si>
+    <t>AssignmentName74026</t>
+  </si>
+  <si>
+    <t>PortfolioCourse81133</t>
+  </si>
+  <si>
+    <t>AssignmentName81133</t>
+  </si>
+  <si>
+    <t>PortfolioCourse5843</t>
+  </si>
+  <si>
+    <t>AssignmentName5843</t>
+  </si>
+  <si>
+    <t>PortfolioCourse85653</t>
+  </si>
+  <si>
+    <t>AssignmentName85653</t>
+  </si>
+  <si>
+    <t>PortfolioCourse38209</t>
+  </si>
+  <si>
+    <t>AssignmentName38209</t>
+  </si>
+  <si>
+    <t>PortfolioCourse19377</t>
+  </si>
+  <si>
+    <t>AssignmentName19377</t>
+  </si>
+  <si>
+    <t>PortfolioCourse19656</t>
+  </si>
+  <si>
+    <t>AssignmentName19656</t>
+  </si>
+  <si>
+    <t>PortfolioCourse96832</t>
+  </si>
+  <si>
+    <t>AssignmentName96832</t>
+  </si>
+  <si>
+    <t>PortfolioCourse6091</t>
+  </si>
+  <si>
+    <t>AssignmentName6091</t>
+  </si>
+  <si>
+    <t>PortfolioCourse74477</t>
+  </si>
+  <si>
+    <t>AssignmentName74477</t>
+  </si>
+  <si>
+    <t>PortfolioCourse22711</t>
+  </si>
+  <si>
+    <t>AssignmentName22711</t>
+  </si>
+  <si>
+    <t>PortfolioCourse37942</t>
+  </si>
+  <si>
+    <t>AssignmentName37942</t>
+  </si>
+  <si>
+    <t>PortfolioCourse83881</t>
+  </si>
+  <si>
+    <t>AssignmentName83881</t>
+  </si>
+  <si>
+    <t>PortfolioCourse80313</t>
+  </si>
+  <si>
+    <t>AssignmentName80313</t>
+  </si>
+  <si>
+    <t>PortfolioCourse23064</t>
+  </si>
+  <si>
+    <t>AssignmentName23064</t>
+  </si>
+  <si>
+    <t>PortfolioCourse44908</t>
+  </si>
+  <si>
+    <t>AssignmentName44908</t>
+  </si>
+  <si>
+    <t>PortfolioCourse58025</t>
+  </si>
+  <si>
+    <t>AssignmentName58025</t>
+  </si>
+  <si>
+    <t>PortfolioCourse83585</t>
+  </si>
+  <si>
+    <t>AssignmentName83585</t>
+  </si>
+  <si>
+    <t>PortfolioCourse42741</t>
+  </si>
+  <si>
+    <t>AssignmentName42741</t>
+  </si>
+  <si>
+    <t>PortfolioCourse43348</t>
+  </si>
+  <si>
+    <t>AssignmentName43348</t>
   </si>
 </sst>
 </file>
@@ -345,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +540,150 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1194,11 +1482,11 @@
       <c r="L2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>55</v>
+      <c r="M2" t="s" s="67">
+        <v>107</v>
+      </c>
+      <c r="N2" t="s" s="68">
+        <v>108</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>56</v>

</xml_diff>